<commit_message>
Published version of manuscript
</commit_message>
<xml_diff>
--- a/Plots/Figures+Tables/Table_Yahara_FitMetrics.xlsx
+++ b/Plots/Figures+Tables/Table_Yahara_FitMetrics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19155" windowHeight="6945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19152" windowHeight="6948"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -341,7 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -394,9 +394,6 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -414,6 +411,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,46 +699,46 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="A3" sqref="A3:J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="29" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="30" t="s">
+      <c r="F3" s="27"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="31"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="27"/>
+      <c r="J3" s="28"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -769,391 +770,391 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="22">
         <v>0.29893383442536697</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="22">
         <v>0.70860028650691798</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="23">
         <v>0.346928791629669</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="18">
         <v>0.804591360177628</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="18">
         <v>3.1679712538651099</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="19">
         <v>0.65182536353795795</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="29">
         <v>0.21103607472916999</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="29">
         <v>0.128962526186852</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="30">
         <v>0.196400687092041</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>2</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="22">
         <v>0.65124718477184496</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="22">
         <v>0.62058876421443299</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="24">
         <v>5.2844291024319298E-2</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="18">
         <v>0.70562264427237897</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="18">
         <v>3.4867513528893301</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="20">
         <v>1.8455722280709099</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="29">
         <v>0.14467025479491</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="29">
         <v>0.19239143537475301</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="31">
         <v>0.25539112086590599</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>3</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="22">
         <v>0.76395736687242199</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="22">
         <v>0.90885182390155494</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="24">
         <v>0.94324455161880705</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="18">
         <v>1.47399021054301</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="18">
         <v>2.6102767369393298</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="20">
         <v>1.7628949131010301</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="29">
         <v>9.7897527341928706E-2</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="29">
         <v>7.3081863038702996E-2</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="31">
         <v>5.52439265093677E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>4</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="22">
         <v>0.80815607934132405</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="22">
         <v>0.93238912653415795</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="24">
         <v>0.91624517287088103</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="18">
         <v>3.51615177962818</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="18">
         <v>3.1846089765891401</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="20">
         <v>1.6087365662969999</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="29">
         <v>0.128687662104607</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="29">
         <v>6.73032454641911E-2</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="31">
         <v>7.8258353801646904E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>5</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="22">
         <v>0.70865603575751401</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="22">
         <v>0.74148793000023405</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="24">
         <v>0.93000588967129805</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="18">
         <v>3.6879169312191098</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="18">
         <v>4.2758214731234201</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="20">
         <v>3.4627594374599999</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="29">
         <v>0.12852024745267099</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="29">
         <v>0.118782225315693</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="31">
         <v>5.32952224504573E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>6</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="22">
         <v>0.76159262463938504</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="22">
         <v>0.86785168659198597</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="24">
         <v>0.96187015229288797</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="18">
         <v>5.97661572268039</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="18">
         <v>4.6561979726226603</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="20">
         <v>5.0653660160152896</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="29">
         <v>0.121701774036129</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="29">
         <v>9.3954182491140001E-2</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="31">
         <v>6.1598716064428703E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>7</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="22">
         <v>0.48103160170938702</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="22">
         <v>0.927175768043764</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="24">
         <v>0.96377431621462994</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="18">
         <v>9.6186561159850399</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="18">
         <v>4.1644458324254199</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="20">
         <v>2.9710109127481501</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="29">
         <v>0.18244764142058301</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="29">
         <v>5.47075450154531E-2</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="31">
         <v>4.4504787472943702E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>8</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="22">
         <v>0.38147280075054901</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="22">
         <v>0.85638136393992104</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="24">
         <v>0.98820251124196501</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="18">
         <v>7.4421339957729096</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="18">
         <v>5.3040164119123698</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="20">
         <v>1.58511589033216</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="29">
         <v>0.225357101708963</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="29">
         <v>7.8174199009052495E-2</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="31">
         <v>2.31773056894292E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>9</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="22">
         <v>0.58046446284638098</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="22">
         <v>0.85502196792200402</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="24">
         <v>0.93861517313419995</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="18">
         <v>5.0441841735906197</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="18">
         <v>4.7579193347278803</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="20">
         <v>1.2542850256962801</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="29">
         <v>0.123815550991665</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="29">
         <v>7.6662882587368295E-2</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13" s="31">
         <v>6.2726984928789795E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>10</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="22">
         <v>0.71415848574018503</v>
       </c>
-      <c r="C14" s="25">
+      <c r="C14" s="22">
         <v>0.80620875392534397</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="24">
         <v>0.94858657993422502</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="18">
         <v>3.2407535156645202</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="18">
         <v>4.8293841982103602</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="20">
         <v>0.83723586248688298</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="29">
         <v>0.12435885609154999</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="29">
         <v>9.4918819568226898E-2</v>
       </c>
-      <c r="J14" s="19">
+      <c r="J14" s="31">
         <v>4.0057710265424401E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>11</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="22">
         <v>0.77456096119325901</v>
       </c>
-      <c r="C15" s="25">
+      <c r="C15" s="22">
         <v>0.79488855578837703</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="24">
         <v>0.79606031506575703</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="18">
         <v>1.8714758855612701</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="18">
         <v>3.7270223181737898</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="20">
         <v>1.5457588196996901</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="29">
         <v>0.115872090570051</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="29">
         <v>0.110646453091231</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="31">
         <v>8.7484912712915405E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>12</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="22">
         <v>-0.27502169401561499</v>
       </c>
-      <c r="C16" s="25">
+      <c r="C16" s="22">
         <v>0.70066022285516705</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="25">
         <v>0.91341532171165296</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="18">
         <v>1.22581387831991</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="18">
         <v>4.0955610821816002</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="21">
         <v>0.297933672197779</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="29">
         <v>0.19767384704006799</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="29">
         <v>0.12035152993867999</v>
       </c>
-      <c r="J16" s="20">
+      <c r="J16" s="32">
         <v>6.4945188778152002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
@@ -1185,7 +1186,7 @@
         <v>2.78573179421399E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="E3:G3"/>

</xml_diff>